<commit_message>
set up for frames extract
</commit_message>
<xml_diff>
--- a/MTL-AQA_dataset_release/Video_List.xlsx
+++ b/MTL-AQA_dataset_release/Video_List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\matlab\action_quality\actions\diving_2\MTL-AQA_dataset_release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpyneni/GT/9)Grad_School/CS 7643/Research/MTL-AQA/MTL-AQA_dataset_release/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09DE509-B32C-8345-AA18-41017EAAE562}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="11190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11020" windowHeight="11200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -413,23 +414,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +442,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -453,7 +454,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -465,7 +466,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -477,7 +478,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -489,7 +490,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -501,7 +502,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -513,7 +514,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -525,7 +526,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -537,7 +538,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -549,7 +550,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>13</v>
       </c>
@@ -561,7 +562,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>14</v>
       </c>
@@ -573,7 +574,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>17</v>
       </c>
@@ -585,7 +586,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>18</v>
       </c>
@@ -597,7 +598,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>22</v>
       </c>
@@ -609,7 +610,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>26</v>
       </c>
@@ -621,7 +622,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -629,7 +630,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
@@ -637,7 +638,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
@@ -645,7 +646,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
@@ -653,7 +654,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -661,7 +662,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -671,21 +672,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>